<commit_message>
minor arc center correction
</commit_message>
<xml_diff>
--- a/03_AD/MHTG/MHTG_RNAV_FINALES.xlsx
+++ b/03_AD/MHTG/MHTG_RNAV_FINALES.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\mxd_versioned\03_AD\MHTG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\MXD_AIP_HONDURAS\03_AD\MHTG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18120" windowHeight="10740" tabRatio="599"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18120" windowHeight="10740" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MHTG 2-39.10 RNAV (RNP) RW20" sheetId="9" r:id="rId1"/>
-    <sheet name="NORTH RNAV (RNP) RWY 02" sheetId="6" r:id="rId2"/>
-    <sheet name="SOUTH RNAV (RNP) RWY 02" sheetId="7" r:id="rId3"/>
+    <sheet name="NORTH1B" sheetId="6" r:id="rId2"/>
+    <sheet name="SOUTH1B" sheetId="7" r:id="rId3"/>
     <sheet name="MHTG RNP2 SID RWY 02" sheetId="1" r:id="rId4"/>
     <sheet name="MHTG RNP2" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'MHTG RNP2 SID RWY 02'!$A$1:$M$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -1101,6 +1101,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1136,6 +1153,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1317,7 +1351,7 @@
   </sheetPr>
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1702,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="18" t="str">
-        <f t="shared" ref="H5:H14" si="0">W7</f>
+        <f t="shared" ref="H7:H14" si="0">W7</f>
         <v>169.9 (169.5)</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -1736,11 +1770,11 @@
         <v>169.52896000000001</v>
       </c>
       <c r="S7" s="12" t="str">
-        <f t="shared" ref="S5:S14" si="1">MID(M6,1,1)</f>
+        <f t="shared" ref="S7:S14" si="1">MID(M6,1,1)</f>
         <v>0</v>
       </c>
       <c r="T7" s="12" t="str">
-        <f t="shared" ref="T5:T14" si="2">MID(M6,3,2)</f>
+        <f t="shared" ref="T7:T14" si="2">MID(M6,3,2)</f>
         <v>20</v>
       </c>
       <c r="U7" s="12">
@@ -1748,11 +1782,11 @@
         <v>-0.33333333333333331</v>
       </c>
       <c r="V7" s="12">
-        <f t="shared" ref="V5:V14" si="3">R7-U7</f>
+        <f t="shared" ref="V7:V14" si="3">R7-U7</f>
         <v>169.86229333333335</v>
       </c>
       <c r="W7" s="12" t="str">
-        <f t="shared" ref="W5:W14" si="4">TEXT(V7,"000.0")&amp;TEXT(R7," (000.0)")</f>
+        <f t="shared" ref="W7:W14" si="4">TEXT(V7,"000.0")&amp;TEXT(R7," (000.0)")</f>
         <v>169.9 (169.5)</v>
       </c>
     </row>
@@ -2375,8 +2409,8 @@
   </sheetPr>
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2391,12 +2425,12 @@
     <col min="8" max="8" width="10.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.75" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.125" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.125" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="16.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.75" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.625" style="1" customWidth="1"/>
     <col min="18" max="18" width="10.875" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="3.5" hidden="1" customWidth="1"/>

</xml_diff>